<commit_message>
[add] shop data excel 수정
</commit_message>
<xml_diff>
--- a/Assets/ExcelDatas/CharacterData.xlsx
+++ b/Assets/ExcelDatas/CharacterData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ProjectGit\My project\Project_Advence\Assets\ExcelDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7073EDF-214C-4C4E-A182-A1FB75F92CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B0A784-12C6-43FA-A3EC-6E61C7A421C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30735" yWindow="2010" windowWidth="24495" windowHeight="11385" activeTab="1" xr2:uid="{3A0FD73B-EE01-4ABF-87A2-83BD2FE71AFC}"/>
   </bookViews>
@@ -377,10 +377,10 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{ED4D281F-14C7-428C-95E7-5FA8F5994F81}" name="Name" dataDxfId="6"/>
     <tableColumn id="8" xr3:uid="{7601506F-6BF0-47B4-AA04-BFFEDDDBECFA}" name="ID" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{43F40881-49B4-4463-9A12-14BD4390D989}" name="UpgradeStatType" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{B780DC8A-64ED-4485-B07C-5DCADC47B51D}" name="Value" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{E23E6074-77E5-4361-AA84-DF1569D359D8}" name="Level" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{C85FF453-1B8E-40F9-8F39-7BD49834E0ED}" name="Price" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{43F40881-49B4-4463-9A12-14BD4390D989}" name="UpgradeStatType" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{B780DC8A-64ED-4485-B07C-5DCADC47B51D}" name="Value" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{E23E6074-77E5-4361-AA84-DF1569D359D8}" name="Level" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{C85FF453-1B8E-40F9-8F39-7BD49834E0ED}" name="Price" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{25616650-F24D-4D72-83F0-33E06FAD29F2}" name="스텟 타입" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -860,7 +860,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -969,7 +969,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3">
-        <v>5001</v>
+        <v>5002</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>28</v>
@@ -992,7 +992,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="3">
-        <v>5001</v>
+        <v>5003</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>28</v>
@@ -1013,7 +1013,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="3">
-        <v>5001</v>
+        <v>5004</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>28</v>
@@ -1034,7 +1034,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="3">
-        <v>5001</v>
+        <v>5005</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>31</v>
@@ -1057,7 +1057,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="3">
-        <v>5001</v>
+        <v>5006</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>31</v>
@@ -1078,7 +1078,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="3">
-        <v>5001</v>
+        <v>5007</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>31</v>

</xml_diff>